<commit_message>
improved excel based game and slot generation tweaked the scheduler logic
</commit_message>
<xml_diff>
--- a/data/TT/Team-2020.xlsx
+++ b/data/TT/Team-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B26312-D323-4BB8-8032-E7C785A95C12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD6E05A-C5A8-40A6-AD2F-C69AAF2E5BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,11 +401,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,10 +1558,10 @@
         <v>81</v>
       </c>
       <c r="D82">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E82">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -1659,20 +1659,6 @@
         <v>6</v>
       </c>
       <c r="E89">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <v>89</v>
-      </c>
-      <c r="D90">
-        <v>6</v>
-      </c>
-      <c r="E90">
         <v>11</v>
       </c>
     </row>

</xml_diff>